<commit_message>
add questions, revise charts on DFM, still putting zero in idiosyncratic lags of target variable unsolved
</commit_message>
<xml_diff>
--- a/ECB_projections.xlsx
+++ b/ECB_projections.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GITHUB\macrometrics-project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32840DDA-B03B-4BF1-A4C0-5F7EED8FF9FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BC0F1C2-DBB1-4754-B906-E38C826B78F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{12C7916D-DF84-4674-81AC-F6E6A0DFF915}"/>
   </bookViews>
@@ -44,7 +44,7 @@
     <t>Mar24MPE</t>
   </si>
   <si>
-    <t>Dec23MPE</t>
+    <t>Dec23BMPE</t>
   </si>
 </sst>
 </file>
@@ -422,14 +422,13 @@
   <dimension ref="B2:D118"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="10.453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.7265625" customWidth="1"/>
-    <col min="4" max="4" width="9.6328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="13" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:4" x14ac:dyDescent="0.35">

</xml_diff>